<commit_message>
Update waiting time chart
</commit_message>
<xml_diff>
--- a/[Compare] Waiting Time.xlsx
+++ b/[Compare] Waiting Time.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MinhPhuong\Desktop\2023-06-01-23-39-26\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minh Phuong\Desktop\Max_min_Fairness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAC6CD3-C679-489F-8CA2-AF1E311BFB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DAA0936-62F6-45ED-A0DA-0FE19276E20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19883,16 +19883,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -19942,16 +19942,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -20922,7 +20922,7 @@
   <dimension ref="A1:B3368"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>